<commit_message>
Fase 1 de validación completa - prueba
</commit_message>
<xml_diff>
--- a/Prevalidador/Tapa OPS .xlsx
+++ b/Prevalidador/Tapa OPS .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indra365-my.sharepoint.com/personal/dacanonm_indracompany_com/Documents/Documentos/GitHub/automatizacion OPS/Prevalidador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9740106F-1614-4473-B123-A727AECFF786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9740106F-1614-4473-B123-A727AECFF786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F476DF8-4A98-44B1-9757-FDD101FDAC52}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{4290F258-20F5-43D0-82F9-9B7EB361A150}">
       <text>
         <r>
           <rPr>
@@ -528,7 +528,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -817,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:P12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1179,7 +1189,10 @@
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="J6:L6"/>
   </mergeCells>
-  <conditionalFormatting sqref="K1:K7">
+  <conditionalFormatting sqref="K1:K6">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>